<commit_message>
All documents revised and completed
</commit_message>
<xml_diff>
--- a/Documentation/Iteration 2/Agile Gantt Chart.xlsx
+++ b/Documentation/Iteration 2/Agile Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{684D94CC-A0DE-4247-869E-2F69DEFAB9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEA6834-D1BA-4E01-BA39-E79748F047D8}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{684D94CC-A0DE-4247-869E-2F69DEFAB9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{495767BB-9058-431F-A2D2-F62A24ED6521}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="415" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="69">
   <si>
     <t>Task 3</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Elisa, Sass</t>
   </si>
   <si>
-    <t>User Acceptance Test Results Template</t>
-  </si>
-  <si>
     <t>ITERATION 3 COMPLETED</t>
   </si>
   <si>
@@ -270,6 +267,18 @@
   </si>
   <si>
     <t>Deploy Timups website</t>
+  </si>
+  <si>
+    <t>Group 6</t>
+  </si>
+  <si>
+    <t>Sass Russell, Elisa Bertoni</t>
+  </si>
+  <si>
+    <t>AGILE PROJECT - E-Commerce Website</t>
+  </si>
+  <si>
+    <t>Manuel User Testing + User Acceptance Test Results Template</t>
   </si>
 </sst>
 </file>
@@ -606,7 +615,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1260,9 +1269,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1302,6 +1308,9 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Accent3" xfId="11" builtinId="37"/>
@@ -1318,6 +1327,36 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="74">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1570,6 +1609,36 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -1813,6 +1882,121 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2075,181 +2259,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.249977111117893"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -2612,9 +2621,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
-          <xdr:colOff>209549</xdr:colOff>
+          <xdr:colOff>220980</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>247650</xdr:rowOff>
+          <xdr:rowOff>236220</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2765,7 +2774,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G35" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G35" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="B9:G35" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2775,12 +2784,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="54" dataCellStyle="Date"/>
-    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="53" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{619BF8F6-D0F1-41AD-871D-FE0240C45A93}" name="Milestone description" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{39BD914E-FB02-4352-846C-6D59624DC0B0}" name="Category" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{D274194F-BCA0-44F3-84B2-217254EE241C}" name="Assigned to" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{8385BC6F-56EE-4363-A106-8DB0A1E4EF5A}" name="Progress" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{02926609-7B93-4B6F-BE96-92EC7A949E4B}" name="Start" dataDxfId="37" dataCellStyle="Date"/>
+    <tableColumn id="6" xr3:uid="{8FF9BE8E-04B7-4B39-AC27-D2E534204BC3}" name="Days" dataDxfId="36" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2792,7 +2801,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0EDB95CA-98FE-4198-8801-690B9B480FDF}" name="Milestones435" displayName="Milestones435" ref="B9:G36" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2802,9 +2811,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{6E47A83D-ACD7-4EB6-9B84-5195E813945E}" name="Milestone description" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{529EEF64-D037-4ACF-8CA4-0C10FE2D1FBB}" name="Category" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{711D01BA-2785-403A-9636-CCC7E2ADA584}" name="Assigned to" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{62B00BEF-16BE-4692-B5E2-F287F680F2C1}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{D6D72902-F68F-4E59-A714-AFFF520C647A}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{93E698DE-286F-49ED-AA20-D0C843671DE8}" name="Days" dataCellStyle="Comma [0]"/>
@@ -2819,7 +2828,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{876EA49D-634E-482B-8173-880F7B761E2C}" name="Milestones43524" displayName="Milestones43524" ref="B9:G36" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B9:G36" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2829,9 +2838,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Assigned to" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{0971B905-713A-4980-8BBC-DF959C2E61F9}" name="Milestone description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4492A0B8-068F-4002-9E8D-E1F5FED367F0}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DF1A764E-7050-4528-B7F9-B6AB99372146}" name="Assigned to" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{47C54592-75B0-4C70-BBF8-0F40483670E9}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{663FB5E0-7616-4EA5-B56A-FF069E2E07D7}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{3B766962-C06F-4E12-BE91-12AB93439874}" name="Days" dataCellStyle="Comma [0]"/>
@@ -3283,8 +3292,8 @@
   </sheetPr>
   <dimension ref="A1:BP37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A23" zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AD26" sqref="AD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="30" customHeight="1"/>
@@ -3305,27 +3314,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="146" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="148"/>
-      <c r="P2" s="148"/>
-      <c r="Q2" s="148"/>
-      <c r="R2" s="148"/>
-      <c r="S2" s="148"/>
-      <c r="T2" s="148"/>
+      <c r="B2" s="159" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="S2" s="147"/>
+      <c r="T2" s="147"/>
       <c r="U2" s="76"/>
       <c r="V2" s="76"/>
       <c r="W2" s="76"/>
@@ -3442,7 +3451,7 @@
     <row r="4" spans="1:68" ht="30" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="81" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="C4" s="82"/>
       <c r="D4" s="83"/>
@@ -3452,26 +3461,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="84"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="99"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="99"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="99"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -3523,7 +3532,7 @@
     <row r="5" spans="1:68" ht="30" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="87" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C5" s="83"/>
       <c r="D5" s="83"/>
@@ -4544,7 +4553,7 @@
     <row r="12" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>8</v>
@@ -4791,7 +4800,7 @@
     <row r="13" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="67" t="s">
         <v>14</v>
@@ -5532,7 +5541,7 @@
     <row r="16" spans="1:68" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="67" t="s">
         <v>16</v>
@@ -5612,7 +5621,7 @@
     <row r="17" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="67" t="s">
         <v>13</v>
@@ -5859,7 +5868,7 @@
     <row r="18" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="67" t="s">
         <v>9</v>
@@ -6344,7 +6353,7 @@
     <row r="20" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="71" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="67" t="s">
         <v>8</v>
@@ -6592,7 +6601,7 @@
     <row r="21" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="67" t="s">
         <v>14</v>
@@ -6840,7 +6849,7 @@
     <row r="22" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="67" t="s">
         <v>14</v>
@@ -7416,7 +7425,7 @@
     <row r="25" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="67" t="s">
         <v>16</v>
@@ -7981,7 +7990,7 @@
     <row r="28" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A28" s="9"/>
       <c r="B28" s="71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="67" t="s">
         <v>8</v>
@@ -8229,7 +8238,7 @@
     <row r="29" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="71" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="67" t="s">
         <v>14</v>
@@ -8479,8 +8488,8 @@
       <c r="B30" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="159" t="s">
-        <v>14</v>
+      <c r="C30" s="158" t="s">
+        <v>13</v>
       </c>
       <c r="D30" s="67" t="s">
         <v>41</v>
@@ -8725,7 +8734,7 @@
     <row r="31" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="67" t="s">
         <v>16</v>
@@ -8805,7 +8814,7 @@
     <row r="32" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C32" s="67" t="s">
         <v>14</v>
@@ -8882,10 +8891,10 @@
       <c r="BL32" s="29"/>
       <c r="BM32" s="21"/>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="60" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="71" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C33" s="67" t="s">
         <v>15</v>
@@ -8901,7 +8910,7 @@
         <v>44699</v>
       </c>
       <c r="G33" s="70">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H33" s="103"/>
       <c r="I33" s="29" t="str">
@@ -9133,7 +9142,7 @@
     <row r="34" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A34" s="9"/>
       <c r="B34" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="67" t="s">
         <v>13</v>
@@ -9213,7 +9222,7 @@
     <row r="35" spans="1:65" s="1" customFormat="1" ht="40.200000000000003" customHeight="1">
       <c r="A35" s="9"/>
       <c r="B35" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="67" t="s">
         <v>9</v>
@@ -9492,39 +9501,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL17 I26:BL35 I19:BL24">
-    <cfRule type="expression" dxfId="44" priority="26">
+    <cfRule type="expression" dxfId="60" priority="26">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="43" priority="29">
+    <cfRule type="expression" dxfId="59" priority="29">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="42" priority="28">
+    <cfRule type="expression" dxfId="58" priority="28">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="41" priority="27">
+    <cfRule type="expression" dxfId="57" priority="27">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL17 I19:BL35">
-    <cfRule type="expression" dxfId="40" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="32" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="33" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="34" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="35" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="36" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9543,24 +9552,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="35" priority="18">
+    <cfRule type="expression" dxfId="51" priority="18">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BL18">
-    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="21" stopIfTrue="1">
       <formula>AND($C18="Low Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="22" stopIfTrue="1">
       <formula>AND($C18="High Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="23" stopIfTrue="1">
       <formula>AND($C18="On Track",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="24" stopIfTrue="1">
       <formula>AND($C18="Med Risk",I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="25" stopIfTrue="1">
       <formula>AND(LEN($C18)=0,I$7&gt;=$F18,I$7&lt;=$F18+$G18-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9579,7 +9588,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25:BL25">
-    <cfRule type="expression" dxfId="29" priority="10">
+    <cfRule type="expression" dxfId="45" priority="10">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9598,7 +9607,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BL32">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="44" priority="2">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9738,6 +9747,21 @@
           <xm:sqref>E31:E32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{41279F5F-57D3-4A88-89E6-B032C7D428E7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="20" id="{B2541656-04BA-42B9-B264-A1E5B0B5D934}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -9813,21 +9837,6 @@
           </x14:cfRule>
           <xm:sqref>I10:BL17 I19:BL24 I26:BL30 I33:BL35</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{41279F5F-57D3-4A88-89E6-B032C7D428E7}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E22</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -9861,27 +9870,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="152"/>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="M2" s="153"/>
-      <c r="N2" s="153"/>
-      <c r="O2" s="154"/>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="155"/>
-      <c r="R2" s="155"/>
-      <c r="S2" s="155"/>
-      <c r="T2" s="155"/>
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="151"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="151"/>
+      <c r="H2" s="151"/>
+      <c r="I2" s="152"/>
+      <c r="J2" s="152"/>
+      <c r="K2" s="152"/>
+      <c r="L2" s="152"/>
+      <c r="M2" s="152"/>
+      <c r="N2" s="152"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
       <c r="U2" s="23"/>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
@@ -10008,26 +10017,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="32"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="35"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="35"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="35"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -17021,56 +17030,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="27" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="25" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="23" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="8" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="10" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="18" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="14" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="15" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17223,27 +17232,27 @@
     <row r="1" spans="1:68" ht="25.2" customHeight="1"/>
     <row r="2" spans="1:68" ht="49.95" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="155" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
-      <c r="L2" s="157"/>
-      <c r="M2" s="157"/>
-      <c r="N2" s="157"/>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
-      <c r="Q2" s="158"/>
-      <c r="R2" s="158"/>
-      <c r="S2" s="158"/>
-      <c r="T2" s="158"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="155"/>
+      <c r="E2" s="155"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="155"/>
+      <c r="H2" s="155"/>
+      <c r="I2" s="156"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="156"/>
+      <c r="L2" s="156"/>
+      <c r="M2" s="156"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="157"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="157"/>
+      <c r="S2" s="157"/>
+      <c r="T2" s="157"/>
       <c r="U2" s="115"/>
       <c r="V2" s="115"/>
       <c r="W2" s="115"/>
@@ -17370,26 +17379,26 @@
         <v>18</v>
       </c>
       <c r="H4" s="84"/>
-      <c r="I4" s="149" t="s">
+      <c r="I4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="149"/>
-      <c r="K4" s="149"/>
-      <c r="L4" s="149"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="148"/>
+      <c r="L4" s="148"/>
       <c r="M4" s="99"/>
-      <c r="N4" s="150" t="s">
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
-      <c r="Q4" s="150"/>
+      <c r="O4" s="149"/>
+      <c r="P4" s="149"/>
+      <c r="Q4" s="149"/>
       <c r="R4" s="99"/>
-      <c r="S4" s="151" t="s">
+      <c r="S4" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="150"/>
+      <c r="V4" s="150"/>
       <c r="W4" s="99"/>
       <c r="X4" s="144" t="s">
         <v>29</v>
@@ -24383,56 +24392,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:AM6">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>I$7&lt;=EOMONTH($I$7,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:BL6">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="15" priority="3">
       <formula>AND(J$7&lt;=EOMONTH($I$7,2),J$7&gt;EOMONTH($I$7,0),J$7&gt;EOMONTH($I$7,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:BL6">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:BL35">
-    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
       <formula>AND($C10="High Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
       <formula>AND($C10="On Track",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>AND($C10="Med Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:BL36">
-    <cfRule type="expression" dxfId="4" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="14" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="15" stopIfTrue="1">
       <formula>AND(#REF!="On Track",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="16" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="17" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24559,6 +24568,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24834,25 +24862,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24863,6 +24872,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24883,18 +24904,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
   <ds:schemaRefs>

</xml_diff>